<commit_message>
fix com port numbers for arrowroot and beet
</commit_message>
<xml_diff>
--- a/protocolRGBms_social_30sec_20190808_low25.xlsx
+++ b/protocolRGBms_social_30sec_20190808_low25.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bransonk\Documents\FlyBubbleParamFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,70 +28,50 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
-    <t xml:space="preserve">Step</t>
+    <t>Step</t>
   </si>
   <si>
-    <t xml:space="preserve">Duration (ms)</t>
+    <t>Duration (ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">Delay(0-120s)</t>
+    <t>Delay(0-120s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Red Intesity  (0-100%)</t>
+    <t>Red Intesity  (0-100%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Pulse Width  (1~180000ms)</t>
+    <t>Pulse Width  (1~180000ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">Pulse Period    (1~180000ms)</t>
+    <t>Pulse Period    (1~180000ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">Pulse Number (1~1000)</t>
+    <t>Pulse Number (1~1000)</t>
   </si>
   <si>
-    <t xml:space="preserve">OffTime   (0-180000ms)</t>
+    <t>OffTime   (0-180000ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">Iteration Number (0~30000)</t>
+    <t>Iteration Number (0~30000)</t>
   </si>
   <si>
-    <t xml:space="preserve">Green Intesity  (0-100%)</t>
+    <t>Green Intesity  (0-100%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Blue Intesity  (0-100%)</t>
+    <t>Blue Intesity  (0-100%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -135,14 +119,14 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -153,7 +137,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -164,7 +148,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -179,7 +163,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -192,11 +176,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
@@ -205,7 +191,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -218,7 +204,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -229,7 +215,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -240,7 +226,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -250,10 +236,12 @@
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -261,192 +249,154 @@
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -505,60 +455,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CF1048576"/>
+  <dimension ref="A1:CF37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="4.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="7.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.85"/>
+    <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="7" style="2" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" customWidth="1"/>
+    <col min="24" max="24" width="6.85546875" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" customWidth="1"/>
+    <col min="29" max="29" width="6" customWidth="1"/>
+    <col min="30" max="30" width="6.42578125" customWidth="1"/>
+    <col min="31" max="31" width="5.42578125" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" customWidth="1"/>
+    <col min="33" max="33" width="23.5703125" customWidth="1"/>
+    <col min="34" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="173.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:84" s="11" customFormat="1" ht="138.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -623,139 +850,139 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="n">
-        <f aca="false">MAX((F2*G2+H2)*I2, (L2*M2+N2)*O2, (R2*S2+T2)*U2) +C3*1000</f>
+      <c r="B2" s="13">
+        <f>MAX((F2*G2+H2)*I2, (L2*M2+N2)*O2, (R2*S2+T2)*U2) +C3*1000</f>
         <v>149994</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="14">
         <v>30</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="15">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="15">
         <v>10</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="15">
         <v>33</v>
       </c>
-      <c r="G2" s="15" t="n">
+      <c r="G2" s="15">
         <v>909</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="15">
         <v>30000</v>
       </c>
-      <c r="I2" s="14" t="n">
+      <c r="I2" s="14">
         <v>2</v>
       </c>
-      <c r="J2" s="15" t="n">
+      <c r="J2" s="15">
         <v>0</v>
       </c>
-      <c r="K2" s="15" t="n">
+      <c r="K2" s="15">
         <v>10</v>
       </c>
-      <c r="L2" s="15" t="n">
+      <c r="L2" s="15">
         <v>33</v>
       </c>
-      <c r="M2" s="15" t="n">
+      <c r="M2" s="15">
         <v>909</v>
       </c>
-      <c r="N2" s="15" t="n">
+      <c r="N2" s="15">
         <v>30000</v>
       </c>
-      <c r="O2" s="14" t="n">
+      <c r="O2" s="14">
         <v>2</v>
       </c>
-      <c r="P2" s="15" t="n">
+      <c r="P2" s="15">
         <v>0</v>
       </c>
-      <c r="Q2" s="15" t="n">
+      <c r="Q2" s="15">
         <v>10</v>
       </c>
-      <c r="R2" s="15" t="n">
+      <c r="R2" s="15">
         <v>33</v>
       </c>
-      <c r="S2" s="15" t="n">
+      <c r="S2" s="15">
         <v>909</v>
       </c>
-      <c r="T2" s="15" t="n">
+      <c r="T2" s="15">
         <v>30000</v>
       </c>
-      <c r="U2" s="14" t="n">
+      <c r="U2" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="n">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="n">
-        <f aca="false">MAX((F3*G3+H3)*I3, (L3*M3+N3)*O3, (R3*S3+T3)*U3) +C4*1000</f>
+      <c r="B3" s="13">
+        <f>MAX((F3*G3+H3)*I3, (L3*M3+N3)*O3, (R3*S3+T3)*U3) +C4*1000</f>
         <v>120000</v>
       </c>
-      <c r="C3" s="17" t="n">
+      <c r="C3" s="17">
         <v>30</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="18">
         <v>5</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="18">
         <v>1000</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="18">
         <v>1000</v>
       </c>
-      <c r="G3" s="18" t="n">
+      <c r="G3" s="18">
         <v>30</v>
       </c>
-      <c r="H3" s="18" t="n">
+      <c r="H3" s="18">
         <v>30000</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="19">
         <v>2</v>
       </c>
-      <c r="J3" s="20" t="n">
+      <c r="J3" s="20">
         <v>0</v>
       </c>
-      <c r="K3" s="18" t="n">
+      <c r="K3" s="18">
         <v>1000</v>
       </c>
-      <c r="L3" s="18" t="n">
+      <c r="L3" s="18">
         <v>1000</v>
       </c>
-      <c r="M3" s="18" t="n">
+      <c r="M3" s="18">
         <v>30</v>
       </c>
-      <c r="N3" s="18" t="n">
+      <c r="N3" s="18">
         <v>30000</v>
       </c>
-      <c r="O3" s="19" t="n">
+      <c r="O3" s="19">
         <v>2</v>
       </c>
-      <c r="P3" s="21" t="n">
+      <c r="P3" s="21">
         <v>0</v>
       </c>
-      <c r="Q3" s="18" t="n">
+      <c r="Q3" s="18">
         <v>1000</v>
       </c>
-      <c r="R3" s="18" t="n">
+      <c r="R3" s="18">
         <v>1000</v>
       </c>
-      <c r="S3" s="18" t="n">
+      <c r="S3" s="18">
         <v>30</v>
       </c>
-      <c r="T3" s="18" t="n">
+      <c r="T3" s="18">
         <v>30000</v>
       </c>
-      <c r="U3" s="19" t="n">
+      <c r="U3" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="4" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -841,7 +1068,7 @@
       <c r="CE4" s="11"/>
       <c r="CF4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -864,7 +1091,7 @@
       <c r="T5" s="21"/>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -887,7 +1114,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="22"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -910,7 +1137,7 @@
       <c r="T7" s="21"/>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -993,7 +1220,7 @@
       <c r="CB8" s="11"/>
       <c r="CC8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1016,7 +1243,7 @@
       <c r="T9" s="21"/>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1039,7 +1266,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="22"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1062,7 +1289,7 @@
       <c r="T11" s="21"/>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1138,7 +1365,7 @@
       <c r="BU12" s="11"/>
       <c r="BV12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -1161,7 +1388,7 @@
       <c r="T13" s="21"/>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1184,7 +1411,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="22"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1208,7 +1435,7 @@
       <c r="U15" s="25"/>
       <c r="Y15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1231,7 +1458,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="22"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1254,7 +1481,7 @@
       <c r="T17" s="21"/>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1277,7 +1504,7 @@
       <c r="T18" s="15"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1300,7 +1527,7 @@
       <c r="T19" s="21"/>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1323,7 +1550,7 @@
       <c r="T20" s="15"/>
       <c r="U20" s="22"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1346,7 +1573,7 @@
       <c r="T21" s="21"/>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1369,7 +1596,7 @@
       <c r="T22" s="14"/>
       <c r="U22" s="22"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1392,7 +1619,7 @@
       <c r="T23" s="21"/>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1415,7 +1642,7 @@
       <c r="T24" s="14"/>
       <c r="U24" s="22"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1438,7 +1665,7 @@
       <c r="T25" s="21"/>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1461,7 +1688,7 @@
       <c r="T26" s="15"/>
       <c r="U26" s="22"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1484,7 +1711,7 @@
       <c r="T27" s="21"/>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1507,7 +1734,7 @@
       <c r="T28" s="14"/>
       <c r="U28" s="22"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1530,7 +1757,7 @@
       <c r="T29" s="21"/>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1553,7 +1780,7 @@
       <c r="T30" s="14"/>
       <c r="U30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1576,7 +1803,7 @@
       <c r="T31" s="21"/>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1599,7 +1826,7 @@
       <c r="T32" s="14"/>
       <c r="U32" s="22"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -1622,7 +1849,7 @@
       <c r="T33" s="21"/>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1645,7 +1872,7 @@
       <c r="T34" s="14"/>
       <c r="U34" s="22"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1668,7 +1895,7 @@
       <c r="T35" s="21"/>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1691,7 +1918,7 @@
       <c r="T36" s="14"/>
       <c r="U36" s="22"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -1714,67 +1941,40 @@
       <c r="T37" s="32"/>
       <c r="U37" s="33"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
+    <col min="1" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
+    <col min="1" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix duration c2 to c3 error in .xlsx, changed the assay to FlyBubbleRGB, made a new shorter debug LED protocol
</commit_message>
<xml_diff>
--- a/protocolRGBms_social_30sec_20190808_low25.xlsx
+++ b/protocolRGBms_social_30sec_20190808_low25.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bransonk\Documents\FlyBubbleParamFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,50 +24,70 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
-    <t>Step</t>
+    <t xml:space="preserve">Step</t>
   </si>
   <si>
-    <t>Duration (ms)</t>
+    <t xml:space="preserve">Duration (ms)</t>
   </si>
   <si>
-    <t>Delay(0-120s)</t>
+    <t xml:space="preserve">Delay(0-120s)</t>
   </si>
   <si>
-    <t>Red Intesity  (0-100%)</t>
+    <t xml:space="preserve">Red Intesity  (0-100%)</t>
   </si>
   <si>
-    <t>Pulse Width  (1~180000ms)</t>
+    <t xml:space="preserve">Pulse Width  (1~180000ms)</t>
   </si>
   <si>
-    <t>Pulse Period    (1~180000ms)</t>
+    <t xml:space="preserve">Pulse Period    (1~180000ms)</t>
   </si>
   <si>
-    <t>Pulse Number (1~1000)</t>
+    <t xml:space="preserve">Pulse Number (1~1000)</t>
   </si>
   <si>
-    <t>OffTime   (0-180000ms)</t>
+    <t xml:space="preserve">OffTime   (0-180000ms)</t>
   </si>
   <si>
-    <t>Iteration Number (0~30000)</t>
+    <t xml:space="preserve">Iteration Number (0~30000)</t>
   </si>
   <si>
-    <t>Green Intesity  (0-100%)</t>
+    <t xml:space="preserve">Green Intesity  (0-100%)</t>
   </si>
   <si>
-    <t>Blue Intesity  (0-100%)</t>
+    <t xml:space="preserve">Blue Intesity  (0-100%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -119,14 +135,14 @@
     </fill>
   </fills>
   <borders count="12">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -137,7 +153,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -148,7 +164,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -163,7 +179,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -176,13 +192,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right style="thin"/>
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
@@ -191,7 +205,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -204,7 +218,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FFD9D9D9"/>
@@ -215,7 +229,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -226,7 +240,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -236,12 +250,10 @@
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
@@ -249,154 +261,192 @@
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFD9D9D9"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right style="thin"/>
       <top style="thin">
         <color rgb="FFD9D9D9"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="34">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -455,337 +505,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:CF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="7" style="2" customWidth="1"/>
-    <col min="21" max="21" width="5.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" customWidth="1"/>
-    <col min="23" max="23" width="6.42578125" customWidth="1"/>
-    <col min="24" max="24" width="6.85546875" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" customWidth="1"/>
-    <col min="29" max="29" width="6" customWidth="1"/>
-    <col min="30" max="30" width="6.42578125" customWidth="1"/>
-    <col min="31" max="31" width="5.42578125" customWidth="1"/>
-    <col min="32" max="32" width="8.85546875" customWidth="1"/>
-    <col min="33" max="33" width="23.5703125" customWidth="1"/>
-    <col min="34" max="1025" width="8.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="4.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="7.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" s="11" customFormat="1" ht="138.75" x14ac:dyDescent="0.25">
+    <row r="1" s="11" customFormat="true" ht="138.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -850,139 +623,139 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
-        <f>MAX((F2*G2+H2)*I2, (L2*M2+N2)*O2, (R2*S2+T2)*U2) +C3*1000</f>
+      <c r="B2" s="13" t="n">
+        <f aca="false">MAX((F2*G2+H2)*I2, (L2*M2+N2)*O2, (R2*S2+T2)*U2) +C2*1000</f>
         <v>149994</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="15" t="n">
         <v>33</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="15" t="n">
         <v>909</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="15" t="n">
         <v>30000</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="15" t="n">
         <v>33</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="15" t="n">
         <v>909</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="15" t="n">
         <v>30000</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="P2" s="15">
+      <c r="P2" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="15" t="n">
         <v>33</v>
       </c>
-      <c r="S2" s="15">
+      <c r="S2" s="15" t="n">
         <v>909</v>
       </c>
-      <c r="T2" s="15">
+      <c r="T2" s="15" t="n">
         <v>30000</v>
       </c>
-      <c r="U2" s="14">
+      <c r="U2" s="14" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="13">
-        <f>MAX((F3*G3+H3)*I3, (L3*M3+N3)*O3, (R3*S3+T3)*U3) +C4*1000</f>
-        <v>120000</v>
-      </c>
-      <c r="C3" s="17">
+      <c r="B3" s="13" t="n">
+        <f aca="false">MAX((F3*G3+H3)*I3, (L3*M3+N3)*O3, (R3*S3+T3)*U3) +C3*1000</f>
+        <v>150000</v>
+      </c>
+      <c r="C3" s="17" t="n">
         <v>30</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="18" t="n">
         <v>30000</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="18" t="n">
         <v>30000</v>
       </c>
-      <c r="O3" s="19">
+      <c r="O3" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="P3" s="21">
+      <c r="P3" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R3" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="S3" s="18">
+      <c r="S3" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="T3" s="18">
+      <c r="T3" s="18" t="n">
         <v>30000</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="19" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1068,7 +841,7 @@
       <c r="CE4" s="11"/>
       <c r="CF4" s="11"/>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1091,7 +864,7 @@
       <c r="T5" s="21"/>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1114,7 +887,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="22"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1137,7 +910,7 @@
       <c r="T7" s="21"/>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1220,7 +993,7 @@
       <c r="CB8" s="11"/>
       <c r="CC8" s="11"/>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1243,7 +1016,7 @@
       <c r="T9" s="21"/>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1266,7 +1039,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="22"/>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1289,7 +1062,7 @@
       <c r="T11" s="21"/>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:84" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1365,7 +1138,7 @@
       <c r="BU12" s="11"/>
       <c r="BV12" s="11"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -1388,7 +1161,7 @@
       <c r="T13" s="21"/>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1411,7 +1184,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="22"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1435,7 +1208,7 @@
       <c r="U15" s="25"/>
       <c r="Y15" s="11"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1458,7 +1231,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="22"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1481,7 +1254,7 @@
       <c r="T17" s="21"/>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1504,7 +1277,7 @@
       <c r="T18" s="15"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1527,7 +1300,7 @@
       <c r="T19" s="21"/>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1550,7 +1323,7 @@
       <c r="T20" s="15"/>
       <c r="U20" s="22"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1573,7 +1346,7 @@
       <c r="T21" s="21"/>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1596,7 +1369,7 @@
       <c r="T22" s="14"/>
       <c r="U22" s="22"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1619,7 +1392,7 @@
       <c r="T23" s="21"/>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1642,7 +1415,7 @@
       <c r="T24" s="14"/>
       <c r="U24" s="22"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1665,7 +1438,7 @@
       <c r="T25" s="21"/>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1688,7 +1461,7 @@
       <c r="T26" s="15"/>
       <c r="U26" s="22"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1711,7 +1484,7 @@
       <c r="T27" s="21"/>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1734,7 +1507,7 @@
       <c r="T28" s="14"/>
       <c r="U28" s="22"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1757,7 +1530,7 @@
       <c r="T29" s="21"/>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1780,7 +1553,7 @@
       <c r="T30" s="14"/>
       <c r="U30" s="22"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1803,7 +1576,7 @@
       <c r="T31" s="21"/>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1826,7 +1599,7 @@
       <c r="T32" s="14"/>
       <c r="U32" s="22"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -1849,7 +1622,7 @@
       <c r="T33" s="21"/>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1872,7 +1645,7 @@
       <c r="T34" s="14"/>
       <c r="U34" s="22"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1895,7 +1668,7 @@
       <c r="T35" s="21"/>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1918,7 +1691,7 @@
       <c r="T36" s="14"/>
       <c r="U36" s="22"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -1942,39 +1715,64 @@
       <c r="U37" s="33"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>